<commit_message>
01.09.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/August/All Detail/31.08.2020/MC Bank Statement August 2020.xlsx
+++ b/2020/August/All Detail/31.08.2020/MC Bank Statement August 2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="August 2020" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Date: 31.08.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -1086,12 +1089,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </bottom>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1540,15 +1547,6 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1588,16 +1586,25 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="44" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1691,7 +1698,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1703,7 +1710,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1726,14 +1733,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2059,21 +2066,21 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="20.25">
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="139" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1">
       <c r="A3" s="42"/>
-      <c r="B3" s="143" t="s">
+      <c r="B3" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="B4" s="43" t="s">
@@ -2188,7 +2195,7 @@
       <c r="C10" s="49">
         <v>1200000</v>
       </c>
-      <c r="D10" s="141">
+      <c r="D10" s="138">
         <v>1200000</v>
       </c>
       <c r="E10" s="48">
@@ -3245,7 +3252,7 @@
   </sheetPr>
   <dimension ref="A1:AL222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -3271,24 +3278,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="26.25">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="146"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="143"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:38" ht="21.75" customHeight="1">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="144" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="149"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="146"/>
       <c r="F2" s="5"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2"/>
@@ -3893,13 +3900,13 @@
       <c r="AL14" s="8"/>
     </row>
     <row r="15" spans="1:38" ht="21.75" customHeight="1">
-      <c r="A15" s="150" t="s">
+      <c r="A15" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="151"/>
-      <c r="C15" s="151"/>
-      <c r="D15" s="151"/>
-      <c r="E15" s="152"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="148"/>
+      <c r="D15" s="148"/>
+      <c r="E15" s="149"/>
       <c r="F15" s="5"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
@@ -10939,65 +10946,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="135" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="135" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="135" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="135" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="135" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="135" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="135" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="135" customWidth="1"/>
     <col min="5" max="5" width="21" style="135" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
     </row>
     <row r="3" spans="1:5" ht="25.5">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="155">
-        <f ca="1">TODAY()</f>
-        <v>44074</v>
-      </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="137"/>
+      <c r="B3" s="156" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="152"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="154"/>
     </row>
     <row r="4" spans="1:5" ht="26.25">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="137" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="140" t="s">
+      <c r="E4" s="137" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11061,14 +11070,18 @@
       </c>
       <c r="E8" s="136"/>
     </row>
+    <row r="11" spans="1:5" ht="60" customHeight="1">
+      <c r="E11" s="135" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>